<commit_message>
Fetch Cell Data based on Rows and Columns Scenario Updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestWorkBook.xlsx
+++ b/src/test/resources/TestWorkBook.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Eclipse_Env\Workspace\Excel_Operations_Handson\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983F5913-57CF-45E4-89F2-07C2CE3432FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648F24BC-5F40-4F90-BD99-0A39FF887740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
+    <sheet name="TestDataSet" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
   <si>
     <t>FirstName</t>
   </si>
@@ -67,6 +68,39 @@
   </si>
   <si>
     <t>BE98765</t>
+  </si>
+  <si>
+    <t>RunMode</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Harry Potter</t>
+  </si>
+  <si>
+    <t>Rupee</t>
+  </si>
+  <si>
+    <t>Account created successfully</t>
+  </si>
+  <si>
+    <t>Hermoine Granger</t>
+  </si>
+  <si>
+    <t>Dollar</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
   </si>
 </sst>
 </file>
@@ -409,9 +443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -478,4 +510,136 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FABFB9BE-FCBA-4C4D-8179-D6BD24F31D5D}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fetch Data Based on Col Name & Suite Runnable Check Scenario Updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestWorkBook.xlsx
+++ b/src/test/resources/TestWorkBook.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Eclipse_Env\Workspace\Excel_Operations_Handson\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648F24BC-5F40-4F90-BD99-0A39FF887740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41452517-740E-4827-9DE9-442A40C20361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
     <sheet name="TestDataSet" sheetId="2" r:id="rId2"/>
+    <sheet name="TestCase" sheetId="3" r:id="rId3"/>
+    <sheet name="TestSuite" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
   <si>
     <t>FirstName</t>
   </si>
@@ -101,6 +103,18 @@
   </si>
   <si>
     <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>Suite</t>
+  </si>
+  <si>
+    <t>BankManagerSuite</t>
+  </si>
+  <si>
+    <t>CustomerSuite</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -443,7 +457,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -516,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FABFB9BE-FCBA-4C4D-8179-D6BD24F31D5D}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,4 +658,58 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0F004E7-1C9C-4B8F-8D9E-2F28187740D7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C04766-3BBF-440C-915F-474B5EEA8CB3}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>